<commit_message>
Modify: adicionando a função de verificar a média no excel
</commit_message>
<xml_diff>
--- a/test/Exemple Test.xlsx
+++ b/test/Exemple Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\Teste-Media-Escolar\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F043DFB9-7B2F-44BD-A0A1-0719D0B02B65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69DDB5-4A3E-4206-983D-81D5FB722341}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{E8F1A71A-23F5-40CF-A639-1B645E1AAAE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Arquivos</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>ValueError("Nota deve estar entre 0 e 10")</t>
+  </si>
+  <si>
+    <t>Verifica_media</t>
+  </si>
+  <si>
+    <t>0 &lt;=  nota &lt;= 5</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
+  </si>
+  <si>
+    <t>Recuperação</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>5 &lt; nota &lt;= 8</t>
+  </si>
+  <si>
+    <t>5 &lt; nota &lt;= 7</t>
+  </si>
+  <si>
+    <t>calcula se o aluno será Aprovado</t>
+  </si>
+  <si>
+    <t>calcula se o aluno ficará em Recuperação</t>
+  </si>
+  <si>
+    <t>calcula se o aluno será Reprovado</t>
   </si>
 </sst>
 </file>
@@ -450,18 +480,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FC4C3-0D19-4888-BCDF-69C18453D2CD}">
-  <dimension ref="B1:F4"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,6 +547,57 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
add: três tests,  verificação de string, verificação de menor que 0 e verificação de maior que 10
</commit_message>
<xml_diff>
--- a/test/Exemple Test.xlsx
+++ b/test/Exemple Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\Teste-Media-Escolar\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69DDB5-4A3E-4206-983D-81D5FB722341}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01E393D-F0FA-42D6-AB55-7C97924857ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{E8F1A71A-23F5-40CF-A639-1B645E1AAAE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Arquivos</t>
   </si>
@@ -54,15 +54,9 @@
     <t>"ola"</t>
   </si>
   <si>
-    <t>TypeError("É necessário que seja um número")</t>
-  </si>
-  <si>
     <t>Enviando um número abaixo de 0 e acima de 10</t>
   </si>
   <si>
-    <t>[-1, 11]</t>
-  </si>
-  <si>
     <t>ValueError("Nota deve estar entre 0 e 10")</t>
   </si>
   <si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>calcula se o aluno será Reprovado</t>
+  </si>
+  <si>
+    <t>TypeError("É necessário que seja um número, strings não inclusas")</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +489,7 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -527,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -538,13 +535,13 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -552,16 +549,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -569,16 +566,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -586,16 +583,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: tests para a funcao calcular media
</commit_message>
<xml_diff>
--- a/test/Exemple Test.xlsx
+++ b/test/Exemple Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\Teste-Media-Escolar\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01E393D-F0FA-42D6-AB55-7C97924857ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFB349D-4EB2-4D4B-8A07-2F2524DEA450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{E8F1A71A-23F5-40CF-A639-1B645E1AAAE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Arquivos</t>
   </si>
@@ -45,52 +45,58 @@
     <t>escola/VerificaMedia.py</t>
   </si>
   <si>
-    <t>Verifica_erro</t>
-  </si>
-  <si>
-    <t>Enviando um str</t>
-  </si>
-  <si>
     <t>"ola"</t>
   </si>
   <si>
-    <t>Enviando um número abaixo de 0 e acima de 10</t>
-  </si>
-  <si>
-    <t>ValueError("Nota deve estar entre 0 e 10")</t>
-  </si>
-  <si>
-    <t>Verifica_media</t>
-  </si>
-  <si>
-    <t>0 &lt;=  nota &lt;= 5</t>
-  </si>
-  <si>
-    <t>Reprovado</t>
-  </si>
-  <si>
-    <t>Recuperação</t>
-  </si>
-  <si>
-    <t>Aprovado</t>
-  </si>
-  <si>
-    <t>5 &lt; nota &lt;= 8</t>
-  </si>
-  <si>
-    <t>5 &lt; nota &lt;= 7</t>
-  </si>
-  <si>
-    <t>calcula se o aluno será Aprovado</t>
-  </si>
-  <si>
-    <t>calcula se o aluno ficará em Recuperação</t>
-  </si>
-  <si>
-    <t>calcula se o aluno será Reprovado</t>
-  </si>
-  <si>
     <t>TypeError("É necessário que seja um número, strings não inclusas")</t>
+  </si>
+  <si>
+    <t>escola/calcularMedia.py</t>
+  </si>
+  <si>
+    <t>Enviando uma string</t>
+  </si>
+  <si>
+    <t>Enviando um número menor que 0</t>
+  </si>
+  <si>
+    <t>Enviando um número maior que 10</t>
+  </si>
+  <si>
+    <t>Enviando uma lista vazia</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>ValueError("it is not allowed to send an empty list")</t>
+  </si>
+  <si>
+    <t>"hi"</t>
+  </si>
+  <si>
+    <t>[1.0, -10.0]</t>
+  </si>
+  <si>
+    <t>ValueError("grades can be from 0 to 10")</t>
+  </si>
+  <si>
+    <t>[1.0, 11.0]</t>
+  </si>
+  <si>
+    <t>Enviando um número abaixo de 0</t>
+  </si>
+  <si>
+    <t>ValueError("Grade must be between 0 and 10")</t>
+  </si>
+  <si>
+    <t>Enviando um número acima de 11</t>
+  </si>
+  <si>
+    <t>calcular_media</t>
+  </si>
+  <si>
+    <t>Verificar_media</t>
   </si>
 </sst>
 </file>
@@ -155,13 +161,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,16 +486,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FC4C3-0D19-4888-BCDF-69C18453D2CD}">
-  <dimension ref="B1:F7"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.5703125" bestFit="1" customWidth="1"/>
@@ -515,16 +524,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -532,16 +541,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
-        <v>-1.1100000000000001</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>-1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -549,30 +558,30 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
@@ -580,19 +589,53 @@
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>